<commit_message>
EPBDS-10183 add more tests for effectiveDate dispatching
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10183_effectiveDate_dispatching.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10183_effectiveDate_dispatching.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\demo\openl-demo\user-workspace\DEFAULT\effDate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diana\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DEDEA1-97C0-48A3-9EAD-AC4801E90CCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23010621-901E-465E-BC58-D91CD43980A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2295" windowWidth="31305" windowHeight="13905" xr2:uid="{D5FE89D3-4CD6-4DAC-A899-32186B92AAC1}"/>
+    <workbookView xWindow="2280" yWindow="1125" windowWidth="28800" windowHeight="12990" xr2:uid="{D5FE89D3-4CD6-4DAC-A899-32186B92AAC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="27">
   <si>
     <t>Spreadsheet Double myRule(Integer a)</t>
   </si>
@@ -60,6 +60,57 @@
   </si>
   <si>
     <t>_res_</t>
+  </si>
+  <si>
+    <t>Spreadsheet Double myRule1 (MyDatatype myDatatype)</t>
+  </si>
+  <si>
+    <t>Datatype MyDatatype</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>currentDate : context</t>
+  </si>
+  <si>
+    <t>Test myRule1 myRule1Test</t>
+  </si>
+  <si>
+    <t>myDatatype.a</t>
+  </si>
+  <si>
+    <t>myDatatype.currentDate</t>
+  </si>
+  <si>
+    <t>Spreadsheet Double myRule3(Integer a)</t>
+  </si>
+  <si>
+    <t>Test myRule3</t>
+  </si>
+  <si>
+    <t>Spreadsheet Double myRule4(Integer a)</t>
+  </si>
+  <si>
+    <t>Test myRule4</t>
+  </si>
+  <si>
+    <t>Spreadsheet Double myRule5(Integer a)</t>
+  </si>
+  <si>
+    <t>Test myRule5</t>
+  </si>
+  <si>
+    <t>expirationDate</t>
+  </si>
+  <si>
+    <t>Spreadsheet Double myRule6(Integer a)</t>
+  </si>
+  <si>
+    <t>Test myRule6</t>
   </si>
 </sst>
 </file>
@@ -96,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -104,10 +155,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -123,9 +191,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,7 +231,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -269,7 +337,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -419,26 +487,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E505013C-044C-457B-9895-921264609CAE}">
-  <dimension ref="E4:G33"/>
+  <dimension ref="B3:AC40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="7" max="7" width="41.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="14.42578125" customWidth="1"/>
+    <col min="29" max="29" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E4" s="6" t="s">
+    <row r="3" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="O3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="J4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="O4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>44075</v>
+      </c>
+      <c r="S4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" s="19">
+        <v>43707</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="X4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y4" s="19">
+        <v>43682</v>
+      </c>
+    </row>
+    <row r="5" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
@@ -448,37 +581,194 @@
       <c r="G5" s="5">
         <v>44048</v>
       </c>
-    </row>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="J5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="9">
+        <v>44048</v>
+      </c>
+      <c r="O5" s="23"/>
+      <c r="P5" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>43682</v>
+      </c>
+      <c r="S5" s="23"/>
+      <c r="T5" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="U5" s="19">
+        <v>43682</v>
+      </c>
+      <c r="W5" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="22"/>
+    </row>
+    <row r="6" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="J6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="O6" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="23"/>
+      <c r="S6" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="T6" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="U6" s="23"/>
+      <c r="W6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="X6" s="21">
+        <v>4</v>
+      </c>
+      <c r="Y6" s="23"/>
+    </row>
+    <row r="7" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="6">
-        <v>5</v>
-      </c>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="21">
+        <v>5</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="J7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="21">
+        <v>5</v>
+      </c>
+      <c r="L7" s="21"/>
+      <c r="O7" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="23"/>
+      <c r="S7" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="T7" s="21">
+        <v>4</v>
+      </c>
+      <c r="U7" s="23"/>
+    </row>
+    <row r="8" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E10" s="6" t="s">
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+    </row>
+    <row r="9" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="O9" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="S9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="W9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="21"/>
+      <c r="AA9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB9" s="21"/>
+      <c r="AC9" s="21"/>
+    </row>
+    <row r="10" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E10" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="J10" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="O10" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>44075</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="U10" s="5">
+        <v>43317</v>
+      </c>
+      <c r="W10" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="X10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y10" s="14">
+        <v>44104</v>
+      </c>
+      <c r="AA10" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC10" s="15">
+        <v>43682</v>
+      </c>
+    </row>
+    <row r="11" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E11" s="4" t="s">
         <v>4</v>
       </c>
@@ -488,33 +778,174 @@
       <c r="G11" s="5">
         <v>43682</v>
       </c>
-    </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="J11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="9">
+        <v>43682</v>
+      </c>
+      <c r="O11" s="23"/>
+      <c r="P11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>43317</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T11" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="U11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>43317</v>
+      </c>
+      <c r="AA11" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="24"/>
+    </row>
+    <row r="12" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="J12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="21"/>
+      <c r="O12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="23"/>
+      <c r="S12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="T12" s="21">
+        <v>3</v>
+      </c>
+      <c r="U12" s="23"/>
+      <c r="W12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="X12" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="23"/>
+      <c r="AA12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="21">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="23"/>
+    </row>
+    <row r="13" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="6">
-        <v>4</v>
-      </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="6" t="s">
+      <c r="F13" s="21">
+        <v>4</v>
+      </c>
+      <c r="G13" s="23"/>
+      <c r="J13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="21">
+        <v>4</v>
+      </c>
+      <c r="L13" s="21"/>
+      <c r="O13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="21">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="23"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="W13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="X13" s="21">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="23"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="21"/>
+      <c r="AC13" s="23"/>
+    </row>
+    <row r="14" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
+      <c r="AC14" s="13"/>
+    </row>
+    <row r="15" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E15" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="J15" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="O15" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="S15" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="W15" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
+      <c r="AA15" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB15" s="21"/>
+      <c r="AC15" s="21"/>
+    </row>
+    <row r="16" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E16" s="4" t="s">
         <v>4</v>
       </c>
@@ -524,33 +955,203 @@
       <c r="G16" s="5">
         <v>43317</v>
       </c>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="J16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="9">
+        <v>43317</v>
+      </c>
+      <c r="O16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>44076</v>
+      </c>
+      <c r="S16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="U16" s="5">
+        <v>42952</v>
+      </c>
+      <c r="W16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y16" s="5">
+        <v>42952</v>
+      </c>
+      <c r="AA16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC16" s="15">
+        <v>44048</v>
+      </c>
+    </row>
+    <row r="17" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="23"/>
+      <c r="J17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="21"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>42952</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T17" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="U17" s="23"/>
+      <c r="W17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="X17" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y17" s="23"/>
+      <c r="AA17" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC17" s="23"/>
+    </row>
+    <row r="18" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="6">
-        <v>3</v>
-      </c>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="6" t="s">
+      <c r="F18" s="21">
+        <v>3</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="J18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="21">
+        <v>3</v>
+      </c>
+      <c r="L18" s="21"/>
+      <c r="O18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="23"/>
+      <c r="S18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="T18" s="21">
+        <v>2</v>
+      </c>
+      <c r="U18" s="23"/>
+      <c r="W18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="X18" s="21">
+        <v>2</v>
+      </c>
+      <c r="Y18" s="23"/>
+      <c r="AA18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB18" s="21">
+        <v>4</v>
+      </c>
+      <c r="AC18" s="23"/>
+    </row>
+    <row r="19" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="O19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P19" s="21">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="23"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="13"/>
+      <c r="AC19" s="13"/>
+    </row>
+    <row r="20" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="AA20" s="13"/>
+      <c r="AB20" s="13"/>
+      <c r="AC20" s="13"/>
+    </row>
+    <row r="21" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E21" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="J21" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="13"/>
+      <c r="AC21" s="13"/>
+    </row>
+    <row r="22" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E22" s="4" t="s">
         <v>4</v>
       </c>
@@ -560,31 +1161,241 @@
       <c r="G22" s="5">
         <v>42952</v>
       </c>
-    </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="J22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L22" s="9">
+        <v>42952</v>
+      </c>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="13"/>
+      <c r="AC22" s="13"/>
+    </row>
+    <row r="23" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="23"/>
+      <c r="J23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" s="21"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="13"/>
+      <c r="AC23" s="13"/>
+    </row>
+    <row r="24" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="6">
-        <v>2</v>
-      </c>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="21">
+        <v>2</v>
+      </c>
+      <c r="G24" s="23"/>
+      <c r="J24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24" s="21">
+        <v>2</v>
+      </c>
+      <c r="L24" s="21"/>
+      <c r="O24" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="S24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="W24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC24" s="13"/>
+    </row>
+    <row r="25" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="O25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA25" s="13"/>
+      <c r="AB25" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC25" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="O26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="U26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="W26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="X26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA26" s="13"/>
+      <c r="AB26" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC26" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="O27" s="5">
+        <v>44049</v>
+      </c>
+      <c r="P27" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>4</v>
+      </c>
+      <c r="S27" s="12">
+        <v>43686</v>
+      </c>
+      <c r="T27" s="7">
+        <v>1</v>
+      </c>
+      <c r="U27" s="7">
+        <v>4</v>
+      </c>
+      <c r="W27" s="5">
+        <v>44049</v>
+      </c>
+      <c r="X27" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="7">
+        <v>4</v>
+      </c>
+      <c r="AA27" s="15"/>
+      <c r="AB27" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="AA28" s="13"/>
+      <c r="AB28" s="13"/>
+      <c r="AC28" s="13"/>
+    </row>
+    <row r="29" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="J30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>7</v>
       </c>
@@ -594,8 +1405,11 @@
       <c r="G31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
         <v>7</v>
       </c>
@@ -605,8 +1419,11 @@
       <c r="G32" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E33" s="5">
         <v>44049</v>
       </c>
@@ -616,11 +1433,93 @@
       <c r="G33">
         <v>5</v>
       </c>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J36" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J38" s="6">
+        <v>1</v>
+      </c>
+      <c r="K38" s="9">
+        <v>44049</v>
+      </c>
+      <c r="L38" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="21"/>
+      <c r="C40" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
+  <mergeCells count="64">
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="W15:Y15"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="W9:Y9"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="T12:U12"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="X12:Y12"/>
+    <mergeCell ref="W10:W11"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="F17:G17"/>
@@ -631,7 +1530,35 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="F12:G12"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="AA9:AC9"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AA15:AC15"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AB11:AC11"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="B40:D40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>